<commit_message>
bottom panel for mobile
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Projects\Critterpedia\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D6578-587A-43FE-8192-F0147DF8A0C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA4AD77-3265-47D9-8112-CC7BDB497395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{1A30D3B5-1059-48BE-A246-3F748EC15229}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="276">
   <si>
     <t>Bitterling</t>
   </si>
@@ -471,6 +471,396 @@
   </si>
   <si>
     <t>1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 0</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>Common Butterfly</t>
+  </si>
+  <si>
+    <t>Flying</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19</t>
+  </si>
+  <si>
+    <t>9 10 11 12 1 2 3 4 5 6</t>
+  </si>
+  <si>
+    <t>Yellow Butterfly</t>
+  </si>
+  <si>
+    <t>3 4 5 6 9 10</t>
+  </si>
+  <si>
+    <t>Tiger Butterfly</t>
+  </si>
+  <si>
+    <t>3 4 5 6 7 8 9</t>
+  </si>
+  <si>
+    <t>Peacock Butterfly</t>
+  </si>
+  <si>
+    <t>3 4 5 6</t>
+  </si>
+  <si>
+    <t>Common Bluebottle</t>
+  </si>
+  <si>
+    <t>Paper Kite Butterfly</t>
+  </si>
+  <si>
+    <t>8 9 10 11 12 13 14 15 16 17 18 19</t>
+  </si>
+  <si>
+    <t>Great Purple Emperor</t>
+  </si>
+  <si>
+    <t>Monach Butterfly</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 9 10 11 12 13 14 15 16 17</t>
+  </si>
+  <si>
+    <t>Emperor Butterfly</t>
+  </si>
+  <si>
+    <t>17 18 19 20 21 22 23 0 1 2 3 4 5 6 7 8</t>
+  </si>
+  <si>
+    <t>6 7 8 9 12 1 2 3</t>
+  </si>
+  <si>
+    <t>Agrias Butterfly</t>
+  </si>
+  <si>
+    <t>8 9 10 11 12 13 14 15 16 17</t>
+  </si>
+  <si>
+    <t>Raja Brooke's Birdwing</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 9 12 1 2</t>
+  </si>
+  <si>
+    <t>Queen Alexandra's Birdwing</t>
+  </si>
+  <si>
+    <t>8 9 10 11 12 13 14 15 16</t>
+  </si>
+  <si>
+    <t>Moth</t>
+  </si>
+  <si>
+    <t>Flying by light</t>
+  </si>
+  <si>
+    <t>19 20 21 22 23 0 1 2 3 4</t>
+  </si>
+  <si>
+    <t>Atlas Moth</t>
+  </si>
+  <si>
+    <t>On trees</t>
+  </si>
+  <si>
+    <t>Madagascan Sunset Moth</t>
+  </si>
+  <si>
+    <t>Long Locust</t>
+  </si>
+  <si>
+    <t>On ground</t>
+  </si>
+  <si>
+    <t>Migratory Locust</t>
+  </si>
+  <si>
+    <t>Rice Grasshopper</t>
+  </si>
+  <si>
+    <t>Grasshopper</t>
+  </si>
+  <si>
+    <t>Cricket</t>
+  </si>
+  <si>
+    <t>Dig at cricket noise</t>
+  </si>
+  <si>
+    <t>Bell Cricket</t>
+  </si>
+  <si>
+    <t>Mantis</t>
+  </si>
+  <si>
+    <t>On flowers</t>
+  </si>
+  <si>
+    <t>Orchid Mantis</t>
+  </si>
+  <si>
+    <t>On white flowers</t>
+  </si>
+  <si>
+    <t>Honeybee</t>
+  </si>
+  <si>
+    <t>Wasp</t>
+  </si>
+  <si>
+    <t>Falls from shaking trees</t>
+  </si>
+  <si>
+    <t>0 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23</t>
+  </si>
+  <si>
+    <t>Brown Cicada</t>
+  </si>
+  <si>
+    <t>7 8</t>
+  </si>
+  <si>
+    <t>Robust Cicada</t>
+  </si>
+  <si>
+    <t>Giant Cicada</t>
+  </si>
+  <si>
+    <t>Walker Cicada</t>
+  </si>
+  <si>
+    <t>Evening Cicada</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 16 17 18 19</t>
+  </si>
+  <si>
+    <t>Cicada Shell</t>
+  </si>
+  <si>
+    <t>Red Dragonfly</t>
+  </si>
+  <si>
+    <t>Darner Dragonfly</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 9 10</t>
+  </si>
+  <si>
+    <t>Banded Dragonfly</t>
+  </si>
+  <si>
+    <t>Damselfly</t>
+  </si>
+  <si>
+    <t>Firefly</t>
+  </si>
+  <si>
+    <t>Mole Cricket</t>
+  </si>
+  <si>
+    <t>Underground</t>
+  </si>
+  <si>
+    <t>11 12 1 2 3 4 5</t>
+  </si>
+  <si>
+    <t>Pondskater</t>
+  </si>
+  <si>
+    <t>Ponds</t>
+  </si>
+  <si>
+    <t>Diving Beetle</t>
+  </si>
+  <si>
+    <t>Ponds and rivers</t>
+  </si>
+  <si>
+    <t>Giant Water Bug</t>
+  </si>
+  <si>
+    <t>19 20 21 22 23 0 1 2 3 4 5 6 7 8</t>
+  </si>
+  <si>
+    <t>Stinkbug</t>
+  </si>
+  <si>
+    <t>Man-faced Stink Bug</t>
+  </si>
+  <si>
+    <t>Ladybug</t>
+  </si>
+  <si>
+    <t>3 4 5 6 10</t>
+  </si>
+  <si>
+    <t>Tiger Beetle</t>
+  </si>
+  <si>
+    <t>2 3 4 5 6 7 8 9 10 11</t>
+  </si>
+  <si>
+    <t>Jewel Beetle</t>
+  </si>
+  <si>
+    <t>Violin Beetle</t>
+  </si>
+  <si>
+    <t>On tree stumps</t>
+  </si>
+  <si>
+    <t>5 6 9 10 11</t>
+  </si>
+  <si>
+    <t>Citrus Long-horned Beetle</t>
+  </si>
+  <si>
+    <t>Rosalia Batesi Beetle</t>
+  </si>
+  <si>
+    <t>Blue Weevil Beetle</t>
+  </si>
+  <si>
+    <t>Dung Beetle</t>
+  </si>
+  <si>
+    <t>Pushing snowballs</t>
+  </si>
+  <si>
+    <t>Earth-boring Dung Beetle</t>
+  </si>
+  <si>
+    <t>Scarab Beetle</t>
+  </si>
+  <si>
+    <t>23 0 1 2 3  4 5 6 7 8</t>
+  </si>
+  <si>
+    <t>Drone Beetle</t>
+  </si>
+  <si>
+    <t>Goliath Beetle</t>
+  </si>
+  <si>
+    <t>Saw Stag</t>
+  </si>
+  <si>
+    <t>Miyama Stag</t>
+  </si>
+  <si>
+    <t>Giant Stag</t>
+  </si>
+  <si>
+    <t>Rainbow Stag</t>
+  </si>
+  <si>
+    <t>Cyclommatus Stag</t>
+  </si>
+  <si>
+    <t>Golden Stag</t>
+  </si>
+  <si>
+    <t>Giraffe Stag</t>
+  </si>
+  <si>
+    <t>Horned Dynastid</t>
+  </si>
+  <si>
+    <t>Horned Atlas</t>
+  </si>
+  <si>
+    <t>Horned Elephant</t>
+  </si>
+  <si>
+    <t>Horned Herucles</t>
+  </si>
+  <si>
+    <t>Walking Stick</t>
+  </si>
+  <si>
+    <t>4 5 6 7 8 17 18 19</t>
+  </si>
+  <si>
+    <t>7 8 9 10 11</t>
+  </si>
+  <si>
+    <t>Walking Leaf</t>
+  </si>
+  <si>
+    <t>Near trees, disguised as furniture leaf</t>
+  </si>
+  <si>
+    <t>Bagworm</t>
+  </si>
+  <si>
+    <t>Ant</t>
+  </si>
+  <si>
+    <t>On rotten food</t>
+  </si>
+  <si>
+    <t>Hermit Crab</t>
+  </si>
+  <si>
+    <t>Beach</t>
+  </si>
+  <si>
+    <t>Wharf Roach</t>
+  </si>
+  <si>
+    <t>On rocks at beach</t>
+  </si>
+  <si>
+    <t>Fly</t>
+  </si>
+  <si>
+    <t>On trash items</t>
+  </si>
+  <si>
+    <t>Mosquito</t>
+  </si>
+  <si>
+    <t>17 18 19 20 21 22 23 0 1 2 3 4</t>
+  </si>
+  <si>
+    <t>Flea</t>
+  </si>
+  <si>
+    <t>On villagers</t>
+  </si>
+  <si>
+    <t>Snail</t>
+  </si>
+  <si>
+    <t>On rocks (raining)</t>
+  </si>
+  <si>
+    <t>Pill Bug</t>
+  </si>
+  <si>
+    <t>Hit rocks</t>
+  </si>
+  <si>
+    <t>23 0 1 2 3 4 5 6  8 9 10 11 12 13 14 15 16</t>
+  </si>
+  <si>
+    <t>Centipede</t>
+  </si>
+  <si>
+    <t>16 17 18 19 20 21 22 23</t>
+  </si>
+  <si>
+    <t>Spider</t>
+  </si>
+  <si>
+    <t>Tarantula</t>
+  </si>
+  <si>
+    <t>Scorpion</t>
   </si>
 </sst>
 </file>
@@ -506,9 +896,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A686ABB-E511-4C9F-AD21-B584F06D28EA}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2909,6 +3300,1765 @@
         <v>144</v>
       </c>
     </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>146</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>147</v>
+      </c>
+      <c r="D82" t="s">
+        <v>148</v>
+      </c>
+      <c r="F82">
+        <v>160</v>
+      </c>
+      <c r="G82" t="s">
+        <v>149</v>
+      </c>
+      <c r="H82" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>151</v>
+      </c>
+      <c r="D83" t="s">
+        <v>148</v>
+      </c>
+      <c r="F83">
+        <v>160</v>
+      </c>
+      <c r="G83" t="s">
+        <v>149</v>
+      </c>
+      <c r="H83" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>146</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>153</v>
+      </c>
+      <c r="D84" t="s">
+        <v>148</v>
+      </c>
+      <c r="F84">
+        <v>240</v>
+      </c>
+      <c r="G84" t="s">
+        <v>149</v>
+      </c>
+      <c r="H84" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>155</v>
+      </c>
+      <c r="D85" t="s">
+        <v>148</v>
+      </c>
+      <c r="F85" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G85" t="s">
+        <v>149</v>
+      </c>
+      <c r="H85" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86" t="s">
+        <v>157</v>
+      </c>
+      <c r="D86" t="s">
+        <v>148</v>
+      </c>
+      <c r="F86">
+        <v>300</v>
+      </c>
+      <c r="G86" t="s">
+        <v>149</v>
+      </c>
+      <c r="H86" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>158</v>
+      </c>
+      <c r="D87" t="s">
+        <v>148</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G87" t="s">
+        <v>159</v>
+      </c>
+      <c r="H87" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>146</v>
+      </c>
+      <c r="B88">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>160</v>
+      </c>
+      <c r="D88" t="s">
+        <v>148</v>
+      </c>
+      <c r="F88" s="2">
+        <v>3000</v>
+      </c>
+      <c r="G88" t="s">
+        <v>149</v>
+      </c>
+      <c r="H88" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D89" t="s">
+        <v>148</v>
+      </c>
+      <c r="F89">
+        <v>140</v>
+      </c>
+      <c r="G89" t="s">
+        <v>162</v>
+      </c>
+      <c r="H89" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>163</v>
+      </c>
+      <c r="D90" t="s">
+        <v>148</v>
+      </c>
+      <c r="F90" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G90" t="s">
+        <v>164</v>
+      </c>
+      <c r="H90" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>146</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" t="s">
+        <v>148</v>
+      </c>
+      <c r="F91" s="2">
+        <v>3000</v>
+      </c>
+      <c r="G91" t="s">
+        <v>167</v>
+      </c>
+      <c r="H91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92">
+        <v>11</v>
+      </c>
+      <c r="C92" t="s">
+        <v>168</v>
+      </c>
+      <c r="D92" t="s">
+        <v>148</v>
+      </c>
+      <c r="F92" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G92" t="s">
+        <v>167</v>
+      </c>
+      <c r="H92" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>146</v>
+      </c>
+      <c r="B93">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>170</v>
+      </c>
+      <c r="D93" t="s">
+        <v>148</v>
+      </c>
+      <c r="F93" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G93" t="s">
+        <v>171</v>
+      </c>
+      <c r="H93" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>146</v>
+      </c>
+      <c r="B94">
+        <v>13</v>
+      </c>
+      <c r="C94" t="s">
+        <v>172</v>
+      </c>
+      <c r="D94" t="s">
+        <v>173</v>
+      </c>
+      <c r="F94">
+        <v>130</v>
+      </c>
+      <c r="G94" t="s">
+        <v>174</v>
+      </c>
+      <c r="H94" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>146</v>
+      </c>
+      <c r="B95">
+        <v>14</v>
+      </c>
+      <c r="C95" t="s">
+        <v>175</v>
+      </c>
+      <c r="D95" t="s">
+        <v>176</v>
+      </c>
+      <c r="F95" s="2">
+        <v>3000</v>
+      </c>
+      <c r="G95" t="s">
+        <v>174</v>
+      </c>
+      <c r="H95" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>146</v>
+      </c>
+      <c r="B96">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>177</v>
+      </c>
+      <c r="D96" t="s">
+        <v>148</v>
+      </c>
+      <c r="F96" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G96" t="s">
+        <v>171</v>
+      </c>
+      <c r="H96" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>146</v>
+      </c>
+      <c r="B97">
+        <v>16</v>
+      </c>
+      <c r="C97" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" t="s">
+        <v>179</v>
+      </c>
+      <c r="F97">
+        <v>200</v>
+      </c>
+      <c r="G97" t="s">
+        <v>159</v>
+      </c>
+      <c r="H97" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>146</v>
+      </c>
+      <c r="B98">
+        <v>17</v>
+      </c>
+      <c r="C98" t="s">
+        <v>180</v>
+      </c>
+      <c r="D98" t="s">
+        <v>179</v>
+      </c>
+      <c r="F98">
+        <v>600</v>
+      </c>
+      <c r="G98" t="s">
+        <v>159</v>
+      </c>
+      <c r="H98" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99">
+        <v>18</v>
+      </c>
+      <c r="C99" t="s">
+        <v>181</v>
+      </c>
+      <c r="D99" t="s">
+        <v>179</v>
+      </c>
+      <c r="F99">
+        <v>160</v>
+      </c>
+      <c r="G99" t="s">
+        <v>159</v>
+      </c>
+      <c r="H99" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>146</v>
+      </c>
+      <c r="B100">
+        <v>19</v>
+      </c>
+      <c r="C100" t="s">
+        <v>182</v>
+      </c>
+      <c r="D100" t="s">
+        <v>179</v>
+      </c>
+      <c r="F100">
+        <v>160</v>
+      </c>
+      <c r="G100" t="s">
+        <v>167</v>
+      </c>
+      <c r="H100" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>146</v>
+      </c>
+      <c r="B101">
+        <v>20</v>
+      </c>
+      <c r="C101" t="s">
+        <v>183</v>
+      </c>
+      <c r="D101" t="s">
+        <v>184</v>
+      </c>
+      <c r="F101">
+        <v>130</v>
+      </c>
+      <c r="G101" t="s">
+        <v>164</v>
+      </c>
+      <c r="H101" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>146</v>
+      </c>
+      <c r="B102">
+        <v>21</v>
+      </c>
+      <c r="C102" t="s">
+        <v>185</v>
+      </c>
+      <c r="D102" t="s">
+        <v>179</v>
+      </c>
+      <c r="F102">
+        <v>430</v>
+      </c>
+      <c r="G102" t="s">
+        <v>164</v>
+      </c>
+      <c r="H102" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103">
+        <v>22</v>
+      </c>
+      <c r="C103" t="s">
+        <v>186</v>
+      </c>
+      <c r="D103" t="s">
+        <v>187</v>
+      </c>
+      <c r="F103">
+        <v>430</v>
+      </c>
+      <c r="G103" t="s">
+        <v>167</v>
+      </c>
+      <c r="H103" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>146</v>
+      </c>
+      <c r="B104">
+        <v>23</v>
+      </c>
+      <c r="C104" t="s">
+        <v>188</v>
+      </c>
+      <c r="D104" t="s">
+        <v>189</v>
+      </c>
+      <c r="F104" s="2">
+        <v>2400</v>
+      </c>
+      <c r="G104" t="s">
+        <v>167</v>
+      </c>
+      <c r="H104" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>146</v>
+      </c>
+      <c r="B105">
+        <v>24</v>
+      </c>
+      <c r="C105" t="s">
+        <v>190</v>
+      </c>
+      <c r="D105" t="s">
+        <v>148</v>
+      </c>
+      <c r="F105">
+        <v>200</v>
+      </c>
+      <c r="G105" t="s">
+        <v>167</v>
+      </c>
+      <c r="H105" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>146</v>
+      </c>
+      <c r="B106">
+        <v>25</v>
+      </c>
+      <c r="C106" t="s">
+        <v>191</v>
+      </c>
+      <c r="D106" t="s">
+        <v>192</v>
+      </c>
+      <c r="F106" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G106" t="s">
+        <v>193</v>
+      </c>
+      <c r="H106" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>146</v>
+      </c>
+      <c r="B107">
+        <v>26</v>
+      </c>
+      <c r="C107" t="s">
+        <v>194</v>
+      </c>
+      <c r="D107" t="s">
+        <v>176</v>
+      </c>
+      <c r="G107" t="s">
+        <v>167</v>
+      </c>
+      <c r="H107" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>146</v>
+      </c>
+      <c r="B108">
+        <v>27</v>
+      </c>
+      <c r="C108" t="s">
+        <v>196</v>
+      </c>
+      <c r="D108" t="s">
+        <v>176</v>
+      </c>
+      <c r="G108" t="s">
+        <v>167</v>
+      </c>
+      <c r="H108" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>146</v>
+      </c>
+      <c r="B109">
+        <v>28</v>
+      </c>
+      <c r="C109" t="s">
+        <v>197</v>
+      </c>
+      <c r="D109" t="s">
+        <v>176</v>
+      </c>
+      <c r="G109" t="s">
+        <v>167</v>
+      </c>
+      <c r="H109" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>146</v>
+      </c>
+      <c r="B110">
+        <v>29</v>
+      </c>
+      <c r="C110" t="s">
+        <v>198</v>
+      </c>
+      <c r="D110" t="s">
+        <v>176</v>
+      </c>
+      <c r="F110">
+        <v>400</v>
+      </c>
+      <c r="G110" t="s">
+        <v>167</v>
+      </c>
+      <c r="H110" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>146</v>
+      </c>
+      <c r="B111">
+        <v>30</v>
+      </c>
+      <c r="C111" t="s">
+        <v>199</v>
+      </c>
+      <c r="D111" t="s">
+        <v>176</v>
+      </c>
+      <c r="G111" t="s">
+        <v>200</v>
+      </c>
+      <c r="H111" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>146</v>
+      </c>
+      <c r="B112">
+        <v>31</v>
+      </c>
+      <c r="C112" t="s">
+        <v>201</v>
+      </c>
+      <c r="D112" t="s">
+        <v>176</v>
+      </c>
+      <c r="G112" t="s">
+        <v>193</v>
+      </c>
+      <c r="H112" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113">
+        <v>32</v>
+      </c>
+      <c r="C113" t="s">
+        <v>202</v>
+      </c>
+      <c r="D113" t="s">
+        <v>148</v>
+      </c>
+      <c r="F113">
+        <v>180</v>
+      </c>
+      <c r="G113" t="s">
+        <v>159</v>
+      </c>
+      <c r="H113" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>146</v>
+      </c>
+      <c r="B114">
+        <v>33</v>
+      </c>
+      <c r="C114" t="s">
+        <v>203</v>
+      </c>
+      <c r="D114" t="s">
+        <v>148</v>
+      </c>
+      <c r="F114">
+        <v>230</v>
+      </c>
+      <c r="G114" t="s">
+        <v>167</v>
+      </c>
+      <c r="H114" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>146</v>
+      </c>
+      <c r="B115">
+        <v>34</v>
+      </c>
+      <c r="C115" t="s">
+        <v>205</v>
+      </c>
+      <c r="D115" t="s">
+        <v>148</v>
+      </c>
+      <c r="F115" s="2">
+        <v>4500</v>
+      </c>
+      <c r="G115" t="s">
+        <v>167</v>
+      </c>
+      <c r="H115" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>146</v>
+      </c>
+      <c r="B116">
+        <v>35</v>
+      </c>
+      <c r="C116" t="s">
+        <v>206</v>
+      </c>
+      <c r="D116" t="s">
+        <v>148</v>
+      </c>
+      <c r="G116" t="s">
+        <v>193</v>
+      </c>
+      <c r="H116" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>146</v>
+      </c>
+      <c r="B117">
+        <v>36</v>
+      </c>
+      <c r="C117" t="s">
+        <v>207</v>
+      </c>
+      <c r="D117" t="s">
+        <v>148</v>
+      </c>
+      <c r="G117" t="s">
+        <v>174</v>
+      </c>
+      <c r="H117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>146</v>
+      </c>
+      <c r="B118">
+        <v>37</v>
+      </c>
+      <c r="C118" t="s">
+        <v>208</v>
+      </c>
+      <c r="D118" t="s">
+        <v>209</v>
+      </c>
+      <c r="F118">
+        <v>500</v>
+      </c>
+      <c r="G118" t="s">
+        <v>193</v>
+      </c>
+      <c r="H118" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>146</v>
+      </c>
+      <c r="B119">
+        <v>38</v>
+      </c>
+      <c r="C119" t="s">
+        <v>211</v>
+      </c>
+      <c r="D119" t="s">
+        <v>212</v>
+      </c>
+      <c r="F119">
+        <v>130</v>
+      </c>
+      <c r="G119" t="s">
+        <v>159</v>
+      </c>
+      <c r="H119" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>146</v>
+      </c>
+      <c r="B120">
+        <v>39</v>
+      </c>
+      <c r="C120" t="s">
+        <v>213</v>
+      </c>
+      <c r="D120" t="s">
+        <v>214</v>
+      </c>
+      <c r="F120">
+        <v>800</v>
+      </c>
+      <c r="G120" t="s">
+        <v>159</v>
+      </c>
+      <c r="H120" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>146</v>
+      </c>
+      <c r="B121">
+        <v>40</v>
+      </c>
+      <c r="C121" t="s">
+        <v>215</v>
+      </c>
+      <c r="D121" t="s">
+        <v>214</v>
+      </c>
+      <c r="F121" s="2">
+        <v>2000</v>
+      </c>
+      <c r="G121" t="s">
+        <v>216</v>
+      </c>
+      <c r="H121" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>146</v>
+      </c>
+      <c r="B122">
+        <v>41</v>
+      </c>
+      <c r="C122" t="s">
+        <v>217</v>
+      </c>
+      <c r="D122" t="s">
+        <v>187</v>
+      </c>
+      <c r="F122">
+        <v>120</v>
+      </c>
+      <c r="G122" t="s">
+        <v>193</v>
+      </c>
+      <c r="H122" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>146</v>
+      </c>
+      <c r="B123">
+        <v>42</v>
+      </c>
+      <c r="C123" t="s">
+        <v>218</v>
+      </c>
+      <c r="D123" t="s">
+        <v>187</v>
+      </c>
+      <c r="F123" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G123" t="s">
+        <v>216</v>
+      </c>
+      <c r="H123" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A124" t="s">
+        <v>146</v>
+      </c>
+      <c r="B124">
+        <v>43</v>
+      </c>
+      <c r="C124" t="s">
+        <v>219</v>
+      </c>
+      <c r="D124" t="s">
+        <v>187</v>
+      </c>
+      <c r="F124">
+        <v>200</v>
+      </c>
+      <c r="G124" t="s">
+        <v>167</v>
+      </c>
+      <c r="H124" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>146</v>
+      </c>
+      <c r="B125">
+        <v>44</v>
+      </c>
+      <c r="C125" t="s">
+        <v>221</v>
+      </c>
+      <c r="D125" t="s">
+        <v>179</v>
+      </c>
+      <c r="F125" s="2">
+        <v>1500</v>
+      </c>
+      <c r="G125" t="s">
+        <v>193</v>
+      </c>
+      <c r="H125" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A126" t="s">
+        <v>146</v>
+      </c>
+      <c r="B126">
+        <v>45</v>
+      </c>
+      <c r="C126" t="s">
+        <v>223</v>
+      </c>
+      <c r="D126" t="s">
+        <v>176</v>
+      </c>
+      <c r="F126" s="2">
+        <v>2400</v>
+      </c>
+      <c r="G126" t="s">
+        <v>193</v>
+      </c>
+      <c r="H126" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>146</v>
+      </c>
+      <c r="B127">
+        <v>46</v>
+      </c>
+      <c r="C127" t="s">
+        <v>224</v>
+      </c>
+      <c r="D127" t="s">
+        <v>225</v>
+      </c>
+      <c r="F127">
+        <v>450</v>
+      </c>
+      <c r="G127" t="s">
+        <v>193</v>
+      </c>
+      <c r="H127" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A128" t="s">
+        <v>146</v>
+      </c>
+      <c r="B128">
+        <v>47</v>
+      </c>
+      <c r="C128" t="s">
+        <v>227</v>
+      </c>
+      <c r="D128" t="s">
+        <v>225</v>
+      </c>
+      <c r="F128">
+        <v>350</v>
+      </c>
+      <c r="G128" t="s">
+        <v>193</v>
+      </c>
+      <c r="H128" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>146</v>
+      </c>
+      <c r="B129">
+        <v>48</v>
+      </c>
+      <c r="C129" t="s">
+        <v>228</v>
+      </c>
+      <c r="D129" t="s">
+        <v>225</v>
+      </c>
+      <c r="F129" s="2">
+        <v>3000</v>
+      </c>
+      <c r="G129" t="s">
+        <v>193</v>
+      </c>
+      <c r="H129" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A130" t="s">
+        <v>146</v>
+      </c>
+      <c r="B130">
+        <v>49</v>
+      </c>
+      <c r="C130" t="s">
+        <v>229</v>
+      </c>
+      <c r="G130" t="s">
+        <v>193</v>
+      </c>
+      <c r="H130" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>146</v>
+      </c>
+      <c r="B131">
+        <v>50</v>
+      </c>
+      <c r="C131" t="s">
+        <v>230</v>
+      </c>
+      <c r="D131" t="s">
+        <v>231</v>
+      </c>
+      <c r="H131" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A132" t="s">
+        <v>146</v>
+      </c>
+      <c r="B132">
+        <v>51</v>
+      </c>
+      <c r="C132" t="s">
+        <v>232</v>
+      </c>
+      <c r="D132" t="s">
+        <v>179</v>
+      </c>
+      <c r="F132">
+        <v>300</v>
+      </c>
+      <c r="G132" t="s">
+        <v>193</v>
+      </c>
+      <c r="H132" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>146</v>
+      </c>
+      <c r="B133">
+        <v>52</v>
+      </c>
+      <c r="C133" t="s">
+        <v>233</v>
+      </c>
+      <c r="D133" t="s">
+        <v>176</v>
+      </c>
+      <c r="G133" t="s">
+        <v>234</v>
+      </c>
+      <c r="H133" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>146</v>
+      </c>
+      <c r="B134">
+        <v>53</v>
+      </c>
+      <c r="C134" t="s">
+        <v>235</v>
+      </c>
+      <c r="D134" t="s">
+        <v>176</v>
+      </c>
+      <c r="G134" t="s">
+        <v>193</v>
+      </c>
+      <c r="H134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>146</v>
+      </c>
+      <c r="B135">
+        <v>54</v>
+      </c>
+      <c r="C135" t="s">
+        <v>236</v>
+      </c>
+      <c r="D135" t="s">
+        <v>176</v>
+      </c>
+      <c r="F135" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G135" t="s">
+        <v>164</v>
+      </c>
+      <c r="H135" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>146</v>
+      </c>
+      <c r="B136">
+        <v>55</v>
+      </c>
+      <c r="C136" t="s">
+        <v>237</v>
+      </c>
+      <c r="D136" t="s">
+        <v>176</v>
+      </c>
+      <c r="G136" t="s">
+        <v>193</v>
+      </c>
+      <c r="H136" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>146</v>
+      </c>
+      <c r="B137">
+        <v>56</v>
+      </c>
+      <c r="C137" t="s">
+        <v>238</v>
+      </c>
+      <c r="D137" t="s">
+        <v>176</v>
+      </c>
+      <c r="G137" t="s">
+        <v>193</v>
+      </c>
+      <c r="H137" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>146</v>
+      </c>
+      <c r="B138">
+        <v>57</v>
+      </c>
+      <c r="C138" t="s">
+        <v>239</v>
+      </c>
+      <c r="D138" t="s">
+        <v>176</v>
+      </c>
+      <c r="G138" t="s">
+        <v>234</v>
+      </c>
+      <c r="H138" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>146</v>
+      </c>
+      <c r="B139">
+        <v>58</v>
+      </c>
+      <c r="C139" t="s">
+        <v>240</v>
+      </c>
+      <c r="D139" t="s">
+        <v>176</v>
+      </c>
+      <c r="F139" s="2">
+        <v>6000</v>
+      </c>
+      <c r="G139" t="s">
+        <v>216</v>
+      </c>
+      <c r="H139" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>146</v>
+      </c>
+      <c r="B140">
+        <v>59</v>
+      </c>
+      <c r="C140" t="s">
+        <v>241</v>
+      </c>
+      <c r="D140" t="s">
+        <v>176</v>
+      </c>
+      <c r="G140" t="s">
+        <v>164</v>
+      </c>
+      <c r="H140" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>146</v>
+      </c>
+      <c r="B141">
+        <v>60</v>
+      </c>
+      <c r="C141" t="s">
+        <v>242</v>
+      </c>
+      <c r="D141" t="s">
+        <v>176</v>
+      </c>
+      <c r="G141" t="s">
+        <v>164</v>
+      </c>
+      <c r="H141" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>146</v>
+      </c>
+      <c r="B142">
+        <v>61</v>
+      </c>
+      <c r="C142" t="s">
+        <v>243</v>
+      </c>
+      <c r="D142" t="s">
+        <v>176</v>
+      </c>
+      <c r="G142" t="s">
+        <v>164</v>
+      </c>
+      <c r="H142" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>146</v>
+      </c>
+      <c r="B143">
+        <v>62</v>
+      </c>
+      <c r="C143" t="s">
+        <v>244</v>
+      </c>
+      <c r="D143" t="s">
+        <v>176</v>
+      </c>
+      <c r="G143" t="s">
+        <v>164</v>
+      </c>
+      <c r="H143" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144">
+        <v>63</v>
+      </c>
+      <c r="C144" t="s">
+        <v>245</v>
+      </c>
+      <c r="D144" t="s">
+        <v>176</v>
+      </c>
+      <c r="G144" t="s">
+        <v>164</v>
+      </c>
+      <c r="H144" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>146</v>
+      </c>
+      <c r="B145">
+        <v>64</v>
+      </c>
+      <c r="C145" t="s">
+        <v>246</v>
+      </c>
+      <c r="D145" t="s">
+        <v>176</v>
+      </c>
+      <c r="G145" t="s">
+        <v>164</v>
+      </c>
+      <c r="H145" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A146" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146">
+        <v>65</v>
+      </c>
+      <c r="C146" t="s">
+        <v>247</v>
+      </c>
+      <c r="D146" t="s">
+        <v>176</v>
+      </c>
+      <c r="G146" t="s">
+        <v>164</v>
+      </c>
+      <c r="H146" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>66</v>
+      </c>
+      <c r="C147" t="s">
+        <v>248</v>
+      </c>
+      <c r="D147" t="s">
+        <v>192</v>
+      </c>
+      <c r="G147" t="s">
+        <v>249</v>
+      </c>
+      <c r="H147" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A148" t="s">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>67</v>
+      </c>
+      <c r="C148" t="s">
+        <v>251</v>
+      </c>
+      <c r="D148" t="s">
+        <v>252</v>
+      </c>
+      <c r="F148">
+        <v>600</v>
+      </c>
+      <c r="G148" t="s">
+        <v>193</v>
+      </c>
+      <c r="H148" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>146</v>
+      </c>
+      <c r="B149">
+        <v>68</v>
+      </c>
+      <c r="C149" t="s">
+        <v>253</v>
+      </c>
+      <c r="D149" t="s">
+        <v>192</v>
+      </c>
+      <c r="F149">
+        <v>600</v>
+      </c>
+      <c r="G149" t="s">
+        <v>193</v>
+      </c>
+      <c r="H149" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A150" t="s">
+        <v>146</v>
+      </c>
+      <c r="B150">
+        <v>69</v>
+      </c>
+      <c r="C150" t="s">
+        <v>254</v>
+      </c>
+      <c r="D150" t="s">
+        <v>255</v>
+      </c>
+      <c r="G150" t="s">
+        <v>193</v>
+      </c>
+      <c r="H150" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>146</v>
+      </c>
+      <c r="B151">
+        <v>70</v>
+      </c>
+      <c r="C151" t="s">
+        <v>256</v>
+      </c>
+      <c r="D151" t="s">
+        <v>257</v>
+      </c>
+      <c r="F151" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G151" t="s">
+        <v>216</v>
+      </c>
+      <c r="H151" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A152" t="s">
+        <v>146</v>
+      </c>
+      <c r="B152">
+        <v>71</v>
+      </c>
+      <c r="C152" t="s">
+        <v>258</v>
+      </c>
+      <c r="D152" t="s">
+        <v>259</v>
+      </c>
+      <c r="F152">
+        <v>200</v>
+      </c>
+      <c r="G152" t="s">
+        <v>193</v>
+      </c>
+      <c r="H152" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
+        <v>146</v>
+      </c>
+      <c r="B153">
+        <v>72</v>
+      </c>
+      <c r="C153" t="s">
+        <v>260</v>
+      </c>
+      <c r="D153" t="s">
+        <v>261</v>
+      </c>
+      <c r="G153" t="s">
+        <v>193</v>
+      </c>
+      <c r="H153" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A154" t="s">
+        <v>146</v>
+      </c>
+      <c r="B154">
+        <v>73</v>
+      </c>
+      <c r="C154" t="s">
+        <v>262</v>
+      </c>
+      <c r="D154" t="s">
+        <v>148</v>
+      </c>
+      <c r="F154">
+        <v>130</v>
+      </c>
+      <c r="G154" t="s">
+        <v>263</v>
+      </c>
+      <c r="H154" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>146</v>
+      </c>
+      <c r="B155">
+        <v>74</v>
+      </c>
+      <c r="C155" t="s">
+        <v>264</v>
+      </c>
+      <c r="D155" t="s">
+        <v>265</v>
+      </c>
+      <c r="G155" t="s">
+        <v>193</v>
+      </c>
+      <c r="H155" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A156" t="s">
+        <v>146</v>
+      </c>
+      <c r="B156">
+        <v>75</v>
+      </c>
+      <c r="C156" t="s">
+        <v>266</v>
+      </c>
+      <c r="D156" t="s">
+        <v>267</v>
+      </c>
+      <c r="F156">
+        <v>250</v>
+      </c>
+      <c r="G156" t="s">
+        <v>193</v>
+      </c>
+      <c r="H156" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>146</v>
+      </c>
+      <c r="B157">
+        <v>76</v>
+      </c>
+      <c r="C157" t="s">
+        <v>268</v>
+      </c>
+      <c r="D157" t="s">
+        <v>269</v>
+      </c>
+      <c r="F157">
+        <v>250</v>
+      </c>
+      <c r="G157" t="s">
+        <v>270</v>
+      </c>
+      <c r="H157" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A158" t="s">
+        <v>146</v>
+      </c>
+      <c r="B158">
+        <v>77</v>
+      </c>
+      <c r="C158" t="s">
+        <v>271</v>
+      </c>
+      <c r="D158" t="s">
+        <v>269</v>
+      </c>
+      <c r="F158">
+        <v>300</v>
+      </c>
+      <c r="G158" t="s">
+        <v>272</v>
+      </c>
+      <c r="H158" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>146</v>
+      </c>
+      <c r="B159">
+        <v>78</v>
+      </c>
+      <c r="C159" t="s">
+        <v>273</v>
+      </c>
+      <c r="D159" t="s">
+        <v>192</v>
+      </c>
+      <c r="F159">
+        <v>480</v>
+      </c>
+      <c r="G159" t="s">
+        <v>216</v>
+      </c>
+      <c r="H159" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A160" t="s">
+        <v>146</v>
+      </c>
+      <c r="B160">
+        <v>79</v>
+      </c>
+      <c r="C160" t="s">
+        <v>274</v>
+      </c>
+      <c r="D160" t="s">
+        <v>179</v>
+      </c>
+      <c r="F160" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G160" t="s">
+        <v>174</v>
+      </c>
+      <c r="H160" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>146</v>
+      </c>
+      <c r="B161">
+        <v>80</v>
+      </c>
+      <c r="C161" t="s">
+        <v>275</v>
+      </c>
+      <c r="D161" t="s">
+        <v>179</v>
+      </c>
+      <c r="F161" s="2">
+        <v>8000</v>
+      </c>
+      <c r="G161" t="s">
+        <v>174</v>
+      </c>
+      <c r="H161" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update incorrect saddled birchir info
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Projects\Critterpedia\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA4AD77-3265-47D9-8112-CC7BDB497395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F195316-139E-4DA3-8E28-EB001DE5726C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{1A30D3B5-1059-48BE-A246-3F748EC15229}"/>
   </bookViews>
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A686ABB-E511-4C9F-AD21-B584F06D28EA}">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2393,7 +2393,7 @@
         <v>110</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
added sort by bells
</commit_message>
<xml_diff>
--- a/src/assets/data.xlsx
+++ b/src/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Projects\Critterpedia\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26664FAC-7A37-477B-B48C-CD57DE0B2C8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63C9C5B-E801-4DF7-ABAF-3C03147ED751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{1A30D3B5-1059-48BE-A246-3F748EC15229}"/>
   </bookViews>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A686ABB-E511-4C9F-AD21-B584F06D28EA}">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1309,7 +1309,7 @@
         <v>46</v>
       </c>
       <c r="F3">
-        <v>900</v>
+        <v>200</v>
       </c>
       <c r="G3" t="s">
         <v>105</v>

</xml_diff>